<commit_message>
created changes for different html imports and created a change for the SKU.
</commit_message>
<xml_diff>
--- a/ShopifyExcel/ShopifyExcel/obj/Release/netcoreapp2.0/PubTmp/Out/wwwroot/test shopify Lauren.xlsx
+++ b/ShopifyExcel/ShopifyExcel/obj/Release/netcoreapp2.0/PubTmp/Out/wwwroot/test shopify Lauren.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carlo\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{771D133F-1EA1-4F29-8A84-D379CEC2F09D}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{572222F6-E05E-4D6A-8BAC-AE6201DEB197}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8985"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="test shopify Lauren" sheetId="1" r:id="rId1"/>
@@ -119,21 +119,16 @@
 	.back{ background: #DA81F5; }
 	div{ ..border-style:dotted; ..border-width:1px; }
 &lt;/style&gt;
-&lt;div class="row back" align="center"&gt; &lt;img class="imgTitle" src=
-                                           "
-                                           https://img.fragrancex.com/images/products/SKU/large/ZIPMTS34RT.jpg
-                                           "&gt;&lt;/div&gt;
+&lt;div class="row back" align="center"&gt; &lt;img class="imgTitle" src="https://img.fragrancex.com/images/products/SKU/large/ZIPMTS34RT.jpg"&gt;&lt;/div&gt;
 &lt;div class="row back" align="center"&gt;
 	&lt;div class="row" align="center"&gt;&lt;font size="8"&gt;&lt;b&gt; Taylors' Store =D &lt;/b&gt;&lt;/font&gt;&lt;/div&gt;
 	&lt;div class="row"&gt;&lt;font size="8"&gt;&lt;b&gt; 
 	Zippo Original Eau De Toilette Spray Refillable (Tester) By Zippo
 	&lt;/b&gt;&lt;/font&gt;&lt;/div&gt;
 	&lt;div class="row"&gt;&lt;font size="5"&gt;
-			&lt;h3&gt;Product description: &lt;/h3&gt;
-			&lt;p&gt;
-			Zippo Original Cologne by Zippo, Make an affluent and sophisticated statement by wearing a fragrance as elegant and refined as you: zippo original. Released in 2010 by zippo fragrances, this scent is destined to become a legendary force with fans of the zippo lighter, and it is packaged in a lighter-shaped bottle to add to the fun of applying it. Opening notes of bergamot and violet leaf give way to a spicy heart of clary sage and pepper that dries down to a base of virginia cedar for a masculine composition you'll enjoy daily.
-			&lt;/p&gt;
-			&lt;/font&gt;
+		&lt;h3&gt;Product description: &lt;/h3&gt;
+		    &lt;p&gt;Zippo Original Cologne by Zippo, Make an affluent and sophisticated statement by wearing a fragrance as elegant and refined as you: zippo original. Released in 2010 by zippo fragrances, this scent is destined to become a legendary force with fans of the zippo lighter, and it is packaged in a lighter-shaped bottle to add to the fun of applying it. Opening notes of bergamot and violet leaf give way to a spicy heart of clary sage and pepper that dries down to a base of virginia cedar for a masculine composition you'll enjoy daily.&lt;/p&gt;
+		&lt;/font&gt;
 	&lt;/div&gt;
 	&lt;div&gt;
 		&lt;font size="5"&gt;
@@ -206,21 +201,16 @@
 	.back{ background: #DA81F5; }
 	div{ ..border-style:dotted; ..border-width:1px; }
 &lt;/style&gt;
-&lt;div class="row back" align="center"&gt; &lt;img class="imgTitle" src=
-                                           "
-                                           https://img.fragrancex.com/images/products/SKU/large/27075.jpg
-                                           "&gt;&lt;/div&gt;
+&lt;div class="row back" align="center"&gt; &lt;img class="imgTitle" src="https://img.fragrancex.com/images/products/SKU/large/27075.jpg"&gt;&lt;/div&gt;
 &lt;div class="row back" align="center"&gt;
 	&lt;div class="row" align="center"&gt;&lt;font size="8"&gt;&lt;b&gt; Taylors' Store =D &lt;/b&gt;&lt;/font&gt;&lt;/div&gt;
 	&lt;div class="row"&gt;&lt;font size="8"&gt;&lt;b&gt; 
 	Zirh Eau De Toilette Spray By Zirh International
 	&lt;/b&gt;&lt;/font&gt;&lt;/div&gt;
 	&lt;div class="row"&gt;&lt;font size="5"&gt;
-			&lt;h3&gt;Product description: &lt;/h3&gt;
-			&lt;p&gt;
-			Zirh Cologne by Zirh International, Zirh cologne for men was launched by zirh international in 2001. Zirh is a fresh and spicy mixture that opens with ginger and nutmeg essences. The middle notes of the scent are lime and mandarin orange.
-			&lt;/p&gt;
-			&lt;/font&gt;
+		&lt;h3&gt;Product description: &lt;/h3&gt;
+		    &lt;p&gt;Zirh Cologne by Zirh International, Zirh cologne for men was launched by zirh international in 2001. Zirh is a fresh and spicy mixture that opens with ginger and nutmeg essences. The middle notes of the scent are lime and mandarin orange.&lt;/p&gt;
+		&lt;/font&gt;
 	&lt;/div&gt;
 	&lt;div&gt;
 		&lt;font size="5"&gt;
@@ -269,21 +259,16 @@
 	.back{ background: #DA81F5; }
 	div{ ..border-style:dotted; ..border-width:1px; }
 &lt;/style&gt;
-&lt;div class="row back" align="center"&gt; &lt;img class="imgTitle" src=
-                                           "
-                                           https://img.fragrancex.com/images/products/SKU/large/27076.jpg
-                                           "&gt;&lt;/div&gt;
+&lt;div class="row back" align="center"&gt; &lt;img class="imgTitle" src="https://img.fragrancex.com/images/products/SKU/large/27076.jpg"&gt;&lt;/div&gt;
 &lt;div class="row back" align="center"&gt;
 	&lt;div class="row" align="center"&gt;&lt;font size="8"&gt;&lt;b&gt; Taylors' Store =D &lt;/b&gt;&lt;/font&gt;&lt;/div&gt;
 	&lt;div class="row"&gt;&lt;font size="8"&gt;&lt;b&gt; 
 	Zirh Eau De Toilette Spray By Zirh International
 	&lt;/b&gt;&lt;/font&gt;&lt;/div&gt;
 	&lt;div class="row"&gt;&lt;font size="5"&gt;
-			&lt;h3&gt;Product description: &lt;/h3&gt;
-			&lt;p&gt;
-			Zirh Cologne by Zirh International, Zirh cologne for men was launched by zirh international in 2001. Zirh is a fresh and spicy mixture that opens with ginger and nutmeg essences. The middle notes of the scent are lime and mandarin orange.
-			&lt;/p&gt;
-			&lt;/font&gt;
+		&lt;h3&gt;Product description: &lt;/h3&gt;
+		    &lt;p&gt;Zirh Cologne by Zirh International, Zirh cologne for men was launched by zirh international in 2001. Zirh is a fresh and spicy mixture that opens with ginger and nutmeg essences. The middle notes of the scent are lime and mandarin orange.&lt;/p&gt;
+		&lt;/font&gt;
 	&lt;/div&gt;
 	&lt;div&gt;
 		&lt;font size="5"&gt;
@@ -332,21 +317,16 @@
 	.back{ background: #DA81F5; }
 	div{ ..border-style:dotted; ..border-width:1px; }
 &lt;/style&gt;
-&lt;div class="row back" align="center"&gt; &lt;img class="imgTitle" src=
-                                           "
-                                           https://img.fragrancex.com/images/products/SKU/large/ZI25TSM.jpg
-                                           "&gt;&lt;/div&gt;
+&lt;div class="row back" align="center"&gt; &lt;img class="imgTitle" src="https://img.fragrancex.com/images/products/SKU/large/ZI25TSM.jpg"&gt;&lt;/div&gt;
 &lt;div class="row back" align="center"&gt;
 	&lt;div class="row" align="center"&gt;&lt;font size="8"&gt;&lt;b&gt; Taylors' Store =D &lt;/b&gt;&lt;/font&gt;&lt;/div&gt;
 	&lt;div class="row"&gt;&lt;font size="8"&gt;&lt;b&gt; 
 	Zirh Ikon Eau De Toilette Spray By Zirh International
 	&lt;/b&gt;&lt;/font&gt;&lt;/div&gt;
 	&lt;div class="row"&gt;&lt;font size="5"&gt;
-			&lt;h3&gt;Product description: &lt;/h3&gt;
-			&lt;p&gt;
-			Zirh Ikon Cologne by Zirh International, The company that understands men's grooming introduces its first fragrance for men, a woody oriental for a man with attitude. Top notes are a spicy blend of cardamom, ginger, davano flowers and lemon. The heart notes consist of black cinnamon, cloves, iris root and french labdanum.
-			&lt;/p&gt;
-			&lt;/font&gt;
+		&lt;h3&gt;Product description: &lt;/h3&gt;
+		    &lt;p&gt;Zirh Ikon Cologne by Zirh International, The company that understands men's grooming introduces its first fragrance for men, a woody oriental for a man with attitude. Top notes are a spicy blend of cardamom, ginger, davano flowers and lemon. The heart notes consist of black cinnamon, cloves, iris root and french labdanum.&lt;/p&gt;
+		&lt;/font&gt;
 	&lt;/div&gt;
 	&lt;div&gt;
 		&lt;font size="5"&gt;
@@ -386,21 +366,16 @@
 	.back{ background: #DA81F5; }
 	div{ ..border-style:dotted; ..border-width:1px; }
 &lt;/style&gt;
-&lt;div class="row back" align="center"&gt; &lt;img class="imgTitle" src=
-                                           "
-                                           https://img.fragrancex.com/images/products/SKU/large/ZIHIKO.jpg
-                                           "&gt;&lt;/div&gt;
+&lt;div class="row back" align="center"&gt; &lt;img class="imgTitle" src="https://img.fragrancex.com/images/products/SKU/large/ZIHIKO.jpg"&gt;&lt;/div&gt;
 &lt;div class="row back" align="center"&gt;
 	&lt;div class="row" align="center"&gt;&lt;font size="8"&gt;&lt;b&gt; Taylors' Store =D &lt;/b&gt;&lt;/font&gt;&lt;/div&gt;
 	&lt;div class="row"&gt;&lt;font size="8"&gt;&lt;b&gt; 
 	Zirh Ikon Eau De Toilette Spray By Zirh International
 	&lt;/b&gt;&lt;/font&gt;&lt;/div&gt;
 	&lt;div class="row"&gt;&lt;font size="5"&gt;
-			&lt;h3&gt;Product description: &lt;/h3&gt;
-			&lt;p&gt;
-			Zirh Ikon Cologne by Zirh International, The company that understands men's grooming introduces its first fragrance for men, a woody oriental for a man with attitude. Top notes are a spicy blend of cardamom, ginger, davano flowers and lemon. The heart notes consist of black cinnamon, cloves, iris root and french labdanum.
-			&lt;/p&gt;
-			&lt;/font&gt;
+		&lt;h3&gt;Product description: &lt;/h3&gt;
+		    &lt;p&gt;Zirh Ikon Cologne by Zirh International, The company that understands men's grooming introduces its first fragrance for men, a woody oriental for a man with attitude. Top notes are a spicy blend of cardamom, ginger, davano flowers and lemon. The heart notes consist of black cinnamon, cloves, iris root and french labdanum.&lt;/p&gt;
+		&lt;/font&gt;
 	&lt;/div&gt;
 	&lt;div&gt;
 		&lt;font size="5"&gt;
@@ -446,21 +421,16 @@
 	.back{ background: #DA81F5; }
 	div{ ..border-style:dotted; ..border-width:1px; }
 &lt;/style&gt;
-&lt;div class="row back" align="center"&gt; &lt;img class="imgTitle" src=
-                                           "
-                                           https://img.fragrancex.com/images/products/SKU/large/ZIVSM.jpg
-                                           "&gt;&lt;/div&gt;
+&lt;div class="row back" align="center"&gt; &lt;img class="imgTitle" src="https://img.fragrancex.com/images/products/SKU/large/ZIVSM.jpg"&gt;&lt;/div&gt;
 &lt;div class="row back" align="center"&gt;
 	&lt;div class="row" align="center"&gt;&lt;font size="8"&gt;&lt;b&gt; Taylors' Store =D &lt;/b&gt;&lt;/font&gt;&lt;/div&gt;
 	&lt;div class="row"&gt;&lt;font size="8"&gt;&lt;b&gt; 
 	Zirh Ikon Vial (sample) By Zirh International
 	&lt;/b&gt;&lt;/font&gt;&lt;/div&gt;
 	&lt;div class="row"&gt;&lt;font size="5"&gt;
-			&lt;h3&gt;Product description: &lt;/h3&gt;
-			&lt;p&gt;
-			Zirh Ikon Cologne by Zirh International, The company that understands men's grooming introduces its first fragrance for men, a woody oriental for a man with attitude. Top notes are a spicy blend of cardamom, ginger, davano flowers and lemon. The heart notes consist of black cinnamon, cloves, iris root and french labdanum.
-			&lt;/p&gt;
-			&lt;/font&gt;
+		&lt;h3&gt;Product description: &lt;/h3&gt;
+		    &lt;p&gt;Zirh Ikon Cologne by Zirh International, The company that understands men's grooming introduces its first fragrance for men, a woody oriental for a man with attitude. Top notes are a spicy blend of cardamom, ginger, davano flowers and lemon. The heart notes consist of black cinnamon, cloves, iris root and french labdanum.&lt;/p&gt;
+		&lt;/font&gt;
 	&lt;/div&gt;
 	&lt;div&gt;
 		&lt;font size="5"&gt;
@@ -512,21 +482,16 @@
 	.back{ background: #DA81F5; }
 	div{ ..border-style:dotted; ..border-width:1px; }
 &lt;/style&gt;
-&lt;div class="row back" align="center"&gt; &lt;img class="imgTitle" src=
-                                           "
-                                           https://img.fragrancex.com/images/products/SKU/large/ZMEDT4.jpg
-                                           "&gt;&lt;/div&gt;
+&lt;div class="row back" align="center"&gt; &lt;img class="imgTitle" src="https://img.fragrancex.com/images/products/SKU/large/ZMEDT4.jpg"&gt;&lt;/div&gt;
 &lt;div class="row back" align="center"&gt;
 	&lt;div class="row" align="center"&gt;&lt;font size="8"&gt;&lt;b&gt; Taylors' Store =D &lt;/b&gt;&lt;/font&gt;&lt;/div&gt;
 	&lt;div class="row"&gt;&lt;font size="8"&gt;&lt;b&gt; 
 	Zizanie Eau De Toilette Spray (unboxed) By Fragonard
 	&lt;/b&gt;&lt;/font&gt;&lt;/div&gt;
 	&lt;div class="row"&gt;&lt;font size="5"&gt;
-			&lt;h3&gt;Product description: &lt;/h3&gt;
-			&lt;p&gt;
-			Zizanie Cologne by Fragonard, Launched by the design house of fragonard in 1932, zizanie is classified as a refined, oriental, woody fragrance. This masculine scent possesses a blend of rich patchouli and sandalwood in a perfect balance.
-			&lt;/p&gt;
-			&lt;/font&gt;
+		&lt;h3&gt;Product description: &lt;/h3&gt;
+		    &lt;p&gt;Zizanie Cologne by Fragonard, Launched by the design house of fragonard in 1932, zizanie is classified as a refined, oriental, woody fragrance. This masculine scent possesses a blend of rich patchouli and sandalwood in a perfect balance.&lt;/p&gt;
+		&lt;/font&gt;
 	&lt;/div&gt;
 	&lt;div&gt;
 		&lt;font size="5"&gt;
@@ -581,21 +546,16 @@
 	.back{ background: #DA81F5; }
 	div{ ..border-style:dotted; ..border-width:1px; }
 &lt;/style&gt;
-&lt;div class="row back" align="center"&gt; &lt;img class="imgTitle" src=
-                                           "
-                                           https://img.fragrancex.com/images/products/SKU/large/ZIZ34WEDT.jpg
-                                           "&gt;&lt;/div&gt;
+&lt;div class="row back" align="center"&gt; &lt;img class="imgTitle" src="https://img.fragrancex.com/images/products/SKU/large/ZIZ34WEDT.jpg"&gt;&lt;/div&gt;
 &lt;div class="row back" align="center"&gt;
 	&lt;div class="row" align="center"&gt;&lt;font size="8"&gt;&lt;b&gt; Taylors' Store =D &lt;/b&gt;&lt;/font&gt;&lt;/div&gt;
 	&lt;div class="row"&gt;&lt;font size="8"&gt;&lt;b&gt; 
 	Zizonia Eau De Toilette Spray By Penhaligon's
 	&lt;/b&gt;&lt;/font&gt;&lt;/div&gt;
 	&lt;div class="row"&gt;&lt;font size="5"&gt;
-			&lt;h3&gt;Product description: &lt;/h3&gt;
-			&lt;p&gt;
-			Zizonia Cologne by Penhaligon's, When you need a subtle fragrance to get your message across, reach for zizonia. This classic scent from penhaligon's is a fitting match for artistic and business-minded men alike. The creamy fragrance begins with a base note of geranium, but citrus hints of orange and bergamot soon emerge.
-			&lt;/p&gt;
-			&lt;/font&gt;
+		&lt;h3&gt;Product description: &lt;/h3&gt;
+		    &lt;p&gt;Zizonia Cologne by Penhaligon's, When you need a subtle fragrance to get your message across, reach for zizonia. This classic scent from penhaligon's is a fitting match for artistic and business-minded men alike. The creamy fragrance begins with a base note of geranium, but citrus hints of orange and bergamot soon emerge.&lt;/p&gt;
+		&lt;/font&gt;
 	&lt;/div&gt;
 	&lt;div&gt;
 		&lt;font size="5"&gt;
@@ -647,21 +607,16 @@
 	.back{ background: #DA81F5; }
 	div{ ..border-style:dotted; ..border-width:1px; }
 &lt;/style&gt;
-&lt;div class="row back" align="center"&gt; &lt;img class="imgTitle" src=
-                                           "
-                                           https://img.fragrancex.com/images/products/SKU/large/ZM34TTM.jpg
-                                           "&gt;&lt;/div&gt;
+&lt;div class="row back" align="center"&gt; &lt;img class="imgTitle" src="https://img.fragrancex.com/images/products/SKU/large/ZM34TTM.jpg"&gt;&lt;/div&gt;
 &lt;div class="row back" align="center"&gt;
 	&lt;div class="row" align="center"&gt;&lt;font size="8"&gt;&lt;b&gt; Taylors' Store =D &lt;/b&gt;&lt;/font&gt;&lt;/div&gt;
 	&lt;div class="row"&gt;&lt;font size="8"&gt;&lt;b&gt; 
 	Zizonia Eau De Toilette Spray (unboxed) By Penhaligon's
 	&lt;/b&gt;&lt;/font&gt;&lt;/div&gt;
 	&lt;div class="row"&gt;&lt;font size="5"&gt;
-			&lt;h3&gt;Product description: &lt;/h3&gt;
-			&lt;p&gt;
-			Zizonia Perfume by Penhaligon's, Zizonia is one of the inimitable fragrances for women by penhaligonâ€™s. It creates a mixture of mysterious, nomadic, and alluring scents that you will surely fall in love with in an instant. It impeccably represents a woman full of elegance, class, and composure with a strong and captivating personality that lies within.
-			&lt;/p&gt;
-			&lt;/font&gt;
+		&lt;h3&gt;Product description: &lt;/h3&gt;
+		    &lt;p&gt;Zizonia Perfume by Penhaligon's, Zizonia is one of the inimitable fragrances for women by penhaligonâ€™s. It creates a mixture of mysterious, nomadic, and alluring scents that you will surely fall in love with in an instant. It impeccably represents a woman full of elegance, class, and composure with a strong and captivating personality that lies within.&lt;/p&gt;
+		&lt;/font&gt;
 	&lt;/div&gt;
 	&lt;div&gt;
 		&lt;font size="5"&gt;
@@ -713,21 +668,16 @@
 	.back{ background: #DA81F5; }
 	div{ ..border-style:dotted; ..border-width:1px; }
 &lt;/style&gt;
-&lt;div class="row back" align="center"&gt; &lt;img class="imgTitle" src=
-                                           "
-                                           https://img.fragrancex.com/images/products/SKU/large/ZOANI33W.jpg
-                                           "&gt;&lt;/div&gt;
+&lt;div class="row back" align="center"&gt; &lt;img class="imgTitle" src="https://img.fragrancex.com/images/products/SKU/large/ZOANI33W.jpg"&gt;&lt;/div&gt;
 &lt;div class="row back" align="center"&gt;
 	&lt;div class="row" align="center"&gt;&lt;font size="8"&gt;&lt;b&gt; Taylors' Store =D &lt;/b&gt;&lt;/font&gt;&lt;/div&gt;
 	&lt;div class="row"&gt;&lt;font size="8"&gt;&lt;b&gt; 
 	Zoa Night Eau De Parfum Spray By Regines
 	&lt;/b&gt;&lt;/font&gt;&lt;/div&gt;
 	&lt;div class="row"&gt;&lt;font size="5"&gt;
-			&lt;h3&gt;Product description: &lt;/h3&gt;
-			&lt;p&gt;
-			Zoa Night Perfume by Regines, Conquer the night when you wear the luscious scent of zoa night perfume. This enticing fragrance for women was introduced by parfums regine in 2009 to celebrate the twentieth anniversary of the brand. Decadent top notes of champagne and lemon verbena lead into floral heart notes including fresh rose, with sensuous base notes of vanilla and amber finishing this memorable perfume.
-			&lt;/p&gt;
-			&lt;/font&gt;
+		&lt;h3&gt;Product description: &lt;/h3&gt;
+		    &lt;p&gt;Zoa Night Perfume by Regines, Conquer the night when you wear the luscious scent of zoa night perfume. This enticing fragrance for women was introduced by parfums regine in 2009 to celebrate the twentieth anniversary of the brand. Decadent top notes of champagne and lemon verbena lead into floral heart notes including fresh rose, with sensuous base notes of vanilla and amber finishing this memorable perfume.&lt;/p&gt;
+		&lt;/font&gt;
 	&lt;/div&gt;
 	&lt;div&gt;
 		&lt;font size="5"&gt;
@@ -769,11 +719,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
-  <fonts count="18">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -908,6 +858,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -1206,7 +1164,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="14" borderId="0"/>
@@ -1241,6 +1199,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="4"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="6"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0"/>
@@ -1250,7 +1209,7 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="9"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0"/>
     <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" fillId="10" applyFill="1" borderId="0" applyBorder="1" xfId="1"/>
     <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" fillId="14" applyFill="1" borderId="0" applyBorder="1" xfId="2"/>
@@ -1285,17 +1244,18 @@
     <xf numFmtId="0" applyNumberFormat="1" fontId="4" applyFont="1" fillId="0" applyFill="1" borderId="2" applyBorder="1" xfId="31"/>
     <xf numFmtId="0" applyNumberFormat="1" fontId="5" applyFont="1" fillId="0" applyFill="1" borderId="3" applyBorder="1" xfId="32"/>
     <xf numFmtId="0" applyNumberFormat="1" fontId="5" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="33"/>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="9" applyFont="1" fillId="5" applyFill="1" borderId="4" applyBorder="1" xfId="34"/>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="12" applyFont="1" fillId="0" applyFill="1" borderId="6" applyBorder="1" xfId="35"/>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="8" applyFont="1" fillId="4" applyFill="1" borderId="0" applyBorder="1" xfId="36"/>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" fillId="8" applyFill="1" borderId="8" applyBorder="1" xfId="37"/>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="10" applyFont="1" fillId="6" applyFill="1" borderId="5" applyBorder="1" xfId="38"/>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="2" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="39"/>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="16" applyFont="1" fillId="0" applyFill="1" borderId="9" applyBorder="1" xfId="40"/>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="14" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="41"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="18" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="34"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="9" applyFont="1" fillId="5" applyFill="1" borderId="4" applyBorder="1" xfId="35"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="12" applyFont="1" fillId="0" applyFill="1" borderId="6" applyBorder="1" xfId="36"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="8" applyFont="1" fillId="4" applyFill="1" borderId="0" applyBorder="1" xfId="37"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" fillId="8" applyFill="1" borderId="8" applyBorder="1" xfId="38"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="10" applyFont="1" fillId="6" applyFill="1" borderId="5" applyBorder="1" xfId="39"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="2" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="40"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="16" applyFont="1" fillId="0" applyFill="1" borderId="9" applyBorder="1" xfId="41"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="14" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="42"/>
     <xf numFmtId="8" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="2" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="3" builtinId="38" customBuiltin="1"/>
@@ -1329,15 +1289,16 @@
     <cellStyle name="Heading 2" xfId="31" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="32" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="33" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="34" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="35" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="36" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="34" builtinId="8"/>
+    <cellStyle name="Input" xfId="35" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="36" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="37" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="37" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="38" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="39" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="40" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="41" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Note" xfId="38" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="39" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="40" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="41" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="42" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1648,16 +1609,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="AB2" sqref="AB2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="45.28515625" customWidth="1"/>
+    <col min="2" max="2" width="62.7109375" customWidth="1"/>
     <col min="3" max="3" width="41.28515625" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" customWidth="1"/>
+    <col min="5" max="5" bestFit="1" width="37" customWidth="1"/>
+    <col min="8" max="8" bestFit="1" width="35" customWidth="1"/>
+    <col min="13" max="13" width="14.42578125" customWidth="1"/>
+    <col min="15" max="15" width="15.42578125" customWidth="1"/>
+    <col min="17" max="17" width="26.85546875" customWidth="1"/>
+    <col min="19" max="19" width="15.5703125" customWidth="1"/>
+    <col min="20" max="20" width="24.85546875" customWidth="1"/>
+    <col min="23" max="23" width="16.42578125" customWidth="1"/>
+    <col min="24" max="24" width="23" customWidth="1"/>
+    <col min="26" max="26" width="27.28515625" customWidth="1"/>
+    <col min="27" max="27" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1786,7 +1761,7 @@
       <c r="R2" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="S2" s="42">
+      <c r="S2" s="43">
         <v>53.14</v>
       </c>
       <c r="U2" s="0" t="b">
@@ -1795,7 +1770,10 @@
       <c r="V2" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="X2" s="0" t="s">
+      <c r="W2" s="0">
+        <v>679602709026</v>
+      </c>
+      <c r="X2" s="34" t="s">
         <v>37</v>
       </c>
       <c r="Z2" s="0" t="s">
@@ -1848,7 +1826,7 @@
       <c r="R3" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="S3" s="42">
+      <c r="S3" s="43">
         <v>29.33</v>
       </c>
       <c r="T3" s="0">
@@ -1859,6 +1837,9 @@
       </c>
       <c r="V3" s="0" t="b">
         <v>0</v>
+      </c>
+      <c r="W3" s="0">
+        <v>679614304097</v>
       </c>
       <c r="X3" s="0" t="s">
         <v>46</v>
@@ -1913,7 +1894,7 @@
       <c r="R4" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="S4" s="42">
+      <c r="S4" s="43">
         <v>34.38</v>
       </c>
       <c r="T4" s="0">
@@ -1924,6 +1905,9 @@
       </c>
       <c r="V4" s="0" t="b">
         <v>0</v>
+      </c>
+      <c r="W4" s="0">
+        <v>679614304080</v>
       </c>
       <c r="X4" s="0" t="s">
         <v>49</v>
@@ -1978,7 +1962,7 @@
       <c r="R5" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="S5" s="42">
+      <c r="S5" s="43">
         <v>30.39</v>
       </c>
       <c r="U5" s="0" t="b">
@@ -1986,6 +1970,9 @@
       </c>
       <c r="V5" s="0" t="b">
         <v>0</v>
+      </c>
+      <c r="W5" s="0">
+        <v>679614350018</v>
       </c>
       <c r="X5" s="0" t="s">
         <v>53</v>
@@ -2040,7 +2027,7 @@
       <c r="R6" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="S6" s="42">
+      <c r="S6" s="43">
         <v>36.41</v>
       </c>
       <c r="T6" s="0">
@@ -2051,6 +2038,9 @@
       </c>
       <c r="V6" s="0" t="b">
         <v>0</v>
+      </c>
+      <c r="W6" s="0">
+        <v>679614350001</v>
       </c>
       <c r="X6" s="0" t="s">
         <v>55</v>
@@ -2105,7 +2095,7 @@
       <c r="R7" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="S7" s="42">
+      <c r="S7" s="43">
         <v>20.53</v>
       </c>
       <c r="U7" s="0" t="b">
@@ -2167,7 +2157,7 @@
       <c r="R8" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="S8" s="42">
+      <c r="S8" s="43">
         <v>61.68</v>
       </c>
       <c r="T8" s="0">
@@ -2232,7 +2222,7 @@
       <c r="R9" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="S9" s="42">
+      <c r="S9" s="43">
         <v>130.43</v>
       </c>
       <c r="T9" s="0">
@@ -2243,6 +2233,9 @@
       </c>
       <c r="V9" s="0" t="b">
         <v>0</v>
+      </c>
+      <c r="W9" s="0">
+        <v>793675001525</v>
       </c>
       <c r="X9" s="0" t="s">
         <v>74</v>
@@ -2297,7 +2290,7 @@
       <c r="R10" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="S10" s="42">
+      <c r="S10" s="43">
         <v>89.99</v>
       </c>
       <c r="U10" s="0" t="b">
@@ -2359,7 +2352,7 @@
       <c r="R11" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="S11" s="42">
+      <c r="S11" s="43">
         <v>42.47</v>
       </c>
       <c r="U11" s="0" t="b">
@@ -2368,6 +2361,9 @@
       <c r="V11" s="0" t="b">
         <v>0</v>
       </c>
+      <c r="W11" s="0">
+        <v>3575070050035</v>
+      </c>
       <c r="X11" s="0" t="s">
         <v>87</v>
       </c>
@@ -2379,6 +2375,9 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="X2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
 </worksheet>

</xml_diff>